<commit_message>
"\dsa" does not work with "\i" --corrected
</commit_message>
<xml_diff>
--- a/2 Udacity BA/Udacity_7_35.xlsx
+++ b/2 Udacity BA/Udacity_7_35.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\#Pyth\#Udacity_BA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\#Git\ReadSQL\2 Udacity BA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{97A97B1C-9552-4514-BB69-9E88ED143E14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B826CD-598A-4951-AF99-A85868F8F084}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{369060FF-BAF0-4430-A3E3-94ADECBF7069}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{369060FF-BAF0-4430-A3E3-94ADECBF7069}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Region</t>
   </si>
@@ -76,6 +76,9 @@
   </si>
   <si>
     <t>Median</t>
+  </si>
+  <si>
+    <t>Skew</t>
   </si>
 </sst>
 </file>
@@ -123,7 +126,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normální" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -139,7 +142,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Motiv Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -435,15 +438,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E4E7D69-DEF5-4D49-8CDD-40691ECE6524}">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,8 +459,11 @@
       <c r="E1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -472,8 +478,12 @@
         <f>MEDIAN(B2:B11)</f>
         <v>366</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2">
+        <f>_xlfn.SKEW.P(B2:B11)</f>
+        <v>1.9969961410460293</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -481,7 +491,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -489,7 +499,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -497,7 +507,7 @@
         <v>278</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -505,7 +515,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -513,7 +523,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -521,7 +531,7 @@
         <v>422</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -529,7 +539,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -537,7 +547,7 @@
         <v>543</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>

</xml_diff>